<commit_message>
ajuste creacion e importacion de nomina
</commit_message>
<xml_diff>
--- a/app/assets/formatsXlsx/Carga_Nomina.xlsx
+++ b/app/assets/formatsXlsx/Carga_Nomina.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\apps\htdocs\tezlikv2\app\assets\formatsXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5A7EAF-6D19-4620-BF76-B49F9D36B67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACE0BE1-BE26-41B4-9144-772C7C0BDCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,6 +48,38 @@
             <family val="2"/>
           </rPr>
           <t>Teenus: Teenus: No modifique los encabezados. Son necesarios al momento de importar los datos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{E29994A4-DF7A-47A0-B062-A624C28038F6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Teenus:
+Nomina:  1
+Servicios: 2
+Manual: 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{DB973A2F-D191-48B1-A799-AF8E48ED5DD8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Teenus:
+Si el tipo de nomina es manual ingrese el valor del porcentaje por ejemplo 40% es igual a 40 de lo contrario ingrese en el campo '1', la plataforma registrara estos datos automaticamente.</t>
         </r>
       </text>
     </comment>
@@ -302,49 +334,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Roboto"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Roboto"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -543,10 +532,53 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -563,19 +595,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:K9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:K9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="nombres_y_apellidos" dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="proceso" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="salario_basico" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="transporte" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="dotaciones" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="horas_extras" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="otros_ingresos" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="horas_trabajo_x_dia" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="dias_trabajo_x_mes" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="tipo_nomina" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="factor" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="nombres_y_apellidos" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="proceso" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="salario_basico" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="transporte" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="dotaciones" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="horas_extras" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="otros_ingresos" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="horas_trabajo_x_dia" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="dias_trabajo_x_mes" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="tipo_nomina" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="factor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -904,21 +936,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>

</xml_diff>